<commit_message>
Completed Testing ofBefore and After suite implementation.
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSources/LoginTest_BeforeTestFail.xlsx
+++ b/src/main/resources/dataSources/LoginTest_BeforeTestFail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14910" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -14,11 +14,12 @@
     <sheet name="AFTER_TEST" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:G21"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -545,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>